<commit_message>
latex om door te sturen naar prof
</commit_message>
<xml_diff>
--- a/data_algoritmes_uitvoeringtests.xlsx
+++ b/data_algoritmes_uitvoeringtests.xlsx
@@ -431,7 +431,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -446,11 +446,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
+              <c:f>Sheet1!$N$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PA-I</c:v>
+                  <c:v>RF(diepte=3)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -487,41 +487,41 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:f>Sheet1!$N$7:$N$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$7:$C$10</c:f>
+              <c:f>Sheet1!$O$7:$O$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>123.2</c:v>
+                  <c:v>21.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.1</c:v>
+                  <c:v>20.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>117.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>114.5</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -532,11 +532,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$5</c:f>
+              <c:f>Sheet1!$S$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>PA-II</c:v>
+                  <c:v>RF(diepte=4)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -573,41 +573,127 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:f>Sheet1!$N$7:$N$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$H$7:$H$10</c:f>
+              <c:f>Sheet1!$T$7:$T$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>116.1</c:v>
+                  <c:v>11.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>115.5</c:v>
+                  <c:v>12.1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>114.6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117</c:v>
+                  <c:v>11.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$X$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>RF(diepte=5)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ffd320"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$N$7:$N$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$7:$Y$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -615,11 +701,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="16996"/>
-        <c:axId val="11882024"/>
+        <c:axId val="61182258"/>
+        <c:axId val="61200873"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="16996"/>
+        <c:axId val="61182258"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -640,7 +726,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t>C</a:t>
+                  <a:t># bomen</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -675,14 +761,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11882024"/>
+        <c:crossAx val="61200873"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11882024"/>
+        <c:axId val="61200873"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -747,7 +833,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16996"/>
+        <c:crossAx val="61182258"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -794,15 +880,14 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -822,11 +907,22 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
@@ -840,7 +936,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -850,7 +946,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$7:$N$10</c:f>
+              <c:f>Sheet1!$S$7:$S$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -870,25 +966,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$O$7:$O$10</c:f>
+              <c:f>Sheet1!$P$7:$P$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>21.4</c:v>
+                  <c:v>87</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>20.1</c:v>
+                  <c:v>91.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>18</c:v>
+                  <c:v>95.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>100.91</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -908,11 +1005,22 @@
             <a:solidFill>
               <a:srgbClr val="ff420e"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
@@ -926,7 +1034,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -936,7 +1044,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$7:$N$10</c:f>
+              <c:f>Sheet1!$S$7:$S$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -956,25 +1064,26 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$7:$T$10</c:f>
+              <c:f>Sheet1!$U$7:$U$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>11.9</c:v>
+                  <c:v>84.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.1</c:v>
+                  <c:v>89.09</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>93.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.7</c:v>
+                  <c:v>98.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -994,11 +1103,22 @@
             <a:solidFill>
               <a:srgbClr val="ffd320"/>
             </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ffd320"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
           <c:dLbls>
             <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
@@ -1012,7 +1132,7 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="outEnd"/>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1022,7 +1142,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$N$7:$N$10</c:f>
+              <c:f>Sheet1!$S$7:$S$10</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -1042,33 +1162,40 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Y$7:$Y$10</c:f>
+              <c:f>Sheet1!$Z$7:$Z$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>84</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.9</c:v>
+                  <c:v>89.6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.7</c:v>
+                  <c:v>93.6</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.3</c:v>
+                  <c:v>98.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="84104275"/>
-        <c:axId val="71384865"/>
-      </c:barChart>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="7843386"/>
+        <c:axId val="20973130"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="84104275"/>
+        <c:axId val="7843386"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1124,16 +1251,17 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71384865"/>
+        <c:crossAx val="20973130"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="71384865"/>
+        <c:axId val="20973130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="80"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1161,7 +1289,7 @@
                   <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
-                  <a:t># keer getrained</a:t>
+                  <a:t>Uitvoeringstijd</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1196,498 +1324,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="84104275"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-              <a:latin typeface="Arial"/>
-            </a:defRPr>
-          </a:pPr>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <c:chart>
-    <c:plotArea>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$N$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RF(diepte=3)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$S$7:$S$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$P$7:$P$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>87</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>91.7</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>95.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100.91</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$S$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RF(diepte=4)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$S$7:$S$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$U$7:$U$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>84.2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89.09</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>93.3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>98.5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$X$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>RF(diepte=5)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ffd320"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="triangle"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ffd320"/>
-              </a:solidFill>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$S$7:$S$10</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$Z$7:$Z$10</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>84</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>89.6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>93.6</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>98.1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:hiLowLines>
-          <c:spPr>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:hiLowLines>
-        <c:marker val="1"/>
-        <c:axId val="57240478"/>
-        <c:axId val="26045612"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="57240478"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t># bomen</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="26045612"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="26045612"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:min val="80"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Uitvoeringstijd</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:latin typeface="Arial"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="57240478"/>
+        <c:crossAx val="7843386"/>
         <c:crossesAt val="1"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1735,7 +1372,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1827,11 +1464,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="17250389"/>
-        <c:axId val="9604173"/>
+        <c:axId val="71413270"/>
+        <c:axId val="72067061"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="17250389"/>
+        <c:axId val="71413270"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1887,14 +1524,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="9604173"/>
+        <c:crossAx val="72067061"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="9604173"/>
+        <c:axId val="72067061"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +1596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="17250389"/>
+        <c:crossAx val="71413270"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2006,7 +1643,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2317,11 +1954,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="23993530"/>
-        <c:axId val="91872632"/>
+        <c:axId val="76150459"/>
+        <c:axId val="26777241"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="23993530"/>
+        <c:axId val="76150459"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2377,14 +2014,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91872632"/>
+        <c:crossAx val="26777241"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="91872632"/>
+        <c:axId val="26777241"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2086,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23993530"/>
+        <c:crossAx val="76150459"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2497,7 +2134,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2606,11 +2243,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="41661973"/>
-        <c:axId val="13358181"/>
+        <c:axId val="61450783"/>
+        <c:axId val="84199096"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="41661973"/>
+        <c:axId val="61450783"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2666,14 +2303,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13358181"/>
+        <c:crossAx val="84199096"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13358181"/>
+        <c:axId val="84199096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2738,7 +2375,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41661973"/>
+        <c:crossAx val="61450783"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2786,7 +2423,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2895,11 +2532,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="1"/>
-        <c:axId val="46117314"/>
-        <c:axId val="86740306"/>
+        <c:axId val="35972644"/>
+        <c:axId val="26325599"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="46117314"/>
+        <c:axId val="35972644"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2955,14 +2592,14 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="86740306"/>
+        <c:crossAx val="26325599"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86740306"/>
+        <c:axId val="26325599"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3027,9 +2664,761 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46117314"/>
+        <c:crossAx val="35972644"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PA-I</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="square"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="004586"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$7:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14.599</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.883</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>13.732</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.314</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PA-II</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="8"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$J$7:$J$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>13.507</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>13.672</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.539</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:axId val="59521615"/>
+        <c:axId val="17407300"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="59521615"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>C</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="17407300"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="17407300"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Gemiddeld mse</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="59521615"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PA-I</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$C$7:$C$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>123.2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>117.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>114.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PA-II</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$B$7:$B$10</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$7:$H$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>116.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>114.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="8840834"/>
+        <c:axId val="61447995"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="8840834"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>C</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="61447995"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="61447995"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t># keer getrained</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="8840834"/>
+        <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3079,16 +3468,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19440</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9360</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>126000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>267480</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>66600</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>373680</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>154800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3096,8 +3485,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3270600" y="2772720"/>
-        <a:ext cx="5937480" cy="3308400"/>
+        <a:off x="126000" y="1886040"/>
+        <a:ext cx="5937120" cy="3308040"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3116,9 +3505,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>19800</xdr:colOff>
+      <xdr:colOff>19440</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>28440</xdr:rowOff>
+      <xdr:rowOff>28080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3127,7 +3516,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10517040" y="2801880"/>
-        <a:ext cx="5758560" cy="3241080"/>
+        <a:ext cx="5758200" cy="3240720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3146,9 +3535,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>315720</xdr:colOff>
+      <xdr:colOff>315360</xdr:colOff>
       <xdr:row>59</xdr:row>
-      <xdr:rowOff>14040</xdr:rowOff>
+      <xdr:rowOff>13680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3157,7 +3546,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="10812960" y="6363360"/>
-        <a:ext cx="5758560" cy="3241440"/>
+        <a:ext cx="5758200" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3176,9 +3565,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>35</xdr:col>
-      <xdr:colOff>500400</xdr:colOff>
+      <xdr:colOff>500040</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>98280</xdr:rowOff>
+      <xdr:rowOff>97920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3187,7 +3576,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="23189760" y="2709000"/>
-        <a:ext cx="5758560" cy="3241440"/>
+        <a:ext cx="5758200" cy="3241080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3206,9 +3595,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>27</xdr:col>
-      <xdr:colOff>478440</xdr:colOff>
+      <xdr:colOff>478080</xdr:colOff>
       <xdr:row>37</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3217,7 +3606,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="16664760" y="2880720"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3236,9 +3625,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>661320</xdr:colOff>
+      <xdr:colOff>660960</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>144000</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3247,7 +3636,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="29037960" y="2754360"/>
-        <a:ext cx="5760720" cy="3241800"/>
+        <a:ext cx="5760360" cy="3241440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3266,9 +3655,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>81360</xdr:colOff>
+      <xdr:colOff>81000</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>145800</xdr:rowOff>
+      <xdr:rowOff>145440</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3277,11 +3666,41 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="24395400" y="6334920"/>
-        <a:ext cx="5759280" cy="3239280"/>
+        <a:ext cx="5758920" cy="3238920"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>767160</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>147960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>23040</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>133200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="767160" y="5512320"/>
+        <a:ext cx="5758200" cy="3236400"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3297,8 +3716,8 @@
   </sheetPr>
   <dimension ref="B5:AG51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Z16" activeCellId="0" sqref="Z16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J42" activeCellId="0" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>